<commit_message>
[KT proj2] -Conclusion remaining
</commit_message>
<xml_diff>
--- a/KTproj2/Reports/Charts.xlsx
+++ b/KTproj2/Reports/Charts.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-160" yWindow="460" windowWidth="38400" windowHeight="21060" tabRatio="500"/>
+    <workbookView xWindow="200" yWindow="460" windowWidth="38400" windowHeight="21060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="22">
   <si>
     <t xml:space="preserve">Kappa </t>
   </si>
@@ -35,16 +35,7 @@
     <t>ROC area</t>
   </si>
   <si>
-    <t>Bayes</t>
-  </si>
-  <si>
-    <t>Tree</t>
-  </si>
-  <si>
     <t>KNN</t>
-  </si>
-  <si>
-    <t>Forest</t>
   </si>
   <si>
     <t>Neg FM</t>
@@ -219,8 +210,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="11">
+  <cellStyleXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -253,17 +248,21 @@
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="11">
+  <cellStyles count="15">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -335,15 +334,7 @@
             </a:r>
             <a:r>
               <a:rPr lang="en-US" altLang="zh-CN" baseline="0"/>
-              <a:t>four</a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="zh-CN" altLang="en-US" baseline="0"/>
-              <a:t> </a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="en-US" altLang="zh-CN" baseline="0"/>
-              <a:t>classifiers</a:t>
+              <a:t>threeclassifiers</a:t>
             </a:r>
             <a:endParaRPr lang="en-US"/>
           </a:p>
@@ -391,11 +382,11 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$N$6</c:f>
+              <c:f>Sheet1!$O$6</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Accuracy </c:v>
+                  <c:v>F-Measure</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -439,7 +430,6 @@
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:dLbls>
-            <c:numFmt formatCode="0.00%" sourceLinked="0"/>
             <c:spPr>
               <a:noFill/>
               <a:ln>
@@ -498,19 +488,16 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$M$7:$M$10</c:f>
+              <c:f>Sheet1!$M$8:$M$10</c:f>
               <c:strCache>
-                <c:ptCount val="4"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>Bayes</c:v>
+                  <c:v>Decision Tree</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Tree</c:v>
+                  <c:v>Random Forest</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>Forest</c:v>
-                </c:pt>
-                <c:pt idx="3">
                   <c:v>KNN</c:v>
                 </c:pt>
               </c:strCache>
@@ -518,21 +505,18 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$N$7:$N$10</c:f>
+              <c:f>Sheet1!$O$8:$O$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>0.55339</c:v>
+                  <c:v>0.593</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.620788</c:v>
+                  <c:v>0.604</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.626472</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.625051</c:v>
+                  <c:v>0.608</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -543,11 +527,11 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$O$6</c:f>
+              <c:f>Sheet1!$P$6</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>F-Measure</c:v>
+                  <c:v>Positive FM</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -649,19 +633,16 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$M$7:$M$10</c:f>
+              <c:f>Sheet1!$M$8:$M$10</c:f>
               <c:strCache>
-                <c:ptCount val="4"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>Bayes</c:v>
+                  <c:v>Decision Tree</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Tree</c:v>
+                  <c:v>Random Forest</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>Forest</c:v>
-                </c:pt>
-                <c:pt idx="3">
                   <c:v>KNN</c:v>
                 </c:pt>
               </c:strCache>
@@ -669,21 +650,18 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$O$7:$O$10</c:f>
+              <c:f>Sheet1!$P$8:$P$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>0.504</c:v>
+                  <c:v>0.456</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.593</c:v>
+                  <c:v>0.435</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.604</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.608</c:v>
+                  <c:v>0.452</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -694,11 +672,11 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$P$6</c:f>
+              <c:f>Sheet1!$Q$6</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Positive FM</c:v>
+                  <c:v>Neg FM</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -800,19 +778,16 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$M$7:$M$10</c:f>
+              <c:f>Sheet1!$M$8:$M$10</c:f>
               <c:strCache>
-                <c:ptCount val="4"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>Bayes</c:v>
+                  <c:v>Decision Tree</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Tree</c:v>
+                  <c:v>Random Forest</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>Forest</c:v>
-                </c:pt>
-                <c:pt idx="3">
                   <c:v>KNN</c:v>
                 </c:pt>
               </c:strCache>
@@ -820,21 +795,18 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$P$7:$P$10</c:f>
+              <c:f>Sheet1!$Q$8:$Q$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>0.322</c:v>
+                  <c:v>0.336</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.456</c:v>
+                  <c:v>0.363</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.435</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.452</c:v>
+                  <c:v>0.375</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -845,11 +817,11 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$Q$6</c:f>
+              <c:f>Sheet1!$R$6</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Neg FM</c:v>
+                  <c:v>Neu FM</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -951,19 +923,16 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$M$7:$M$10</c:f>
+              <c:f>Sheet1!$M$8:$M$10</c:f>
               <c:strCache>
-                <c:ptCount val="4"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>Bayes</c:v>
+                  <c:v>Decision Tree</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Tree</c:v>
+                  <c:v>Random Forest</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>Forest</c:v>
-                </c:pt>
-                <c:pt idx="3">
                   <c:v>KNN</c:v>
                 </c:pt>
               </c:strCache>
@@ -971,171 +940,17 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$Q$7:$Q$10</c:f>
+              <c:f>Sheet1!$R$8:$R$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>0.14</c:v>
+                  <c:v>0.321</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.336</c:v>
+                  <c:v>0.319</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.363</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.375</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:ser>
-          <c:idx val="4"/>
-          <c:order val="4"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$R$6</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Neu FM</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:gradFill rotWithShape="1">
-              <a:gsLst>
-                <a:gs pos="0">
-                  <a:schemeClr val="accent5">
-                    <a:lumMod val="110000"/>
-                    <a:satMod val="105000"/>
-                    <a:tint val="67000"/>
-                  </a:schemeClr>
-                </a:gs>
-                <a:gs pos="50000">
-                  <a:schemeClr val="accent5">
-                    <a:lumMod val="105000"/>
-                    <a:satMod val="103000"/>
-                    <a:tint val="73000"/>
-                  </a:schemeClr>
-                </a:gs>
-                <a:gs pos="100000">
-                  <a:schemeClr val="accent5">
-                    <a:lumMod val="105000"/>
-                    <a:satMod val="109000"/>
-                    <a:tint val="81000"/>
-                  </a:schemeClr>
-                </a:gs>
-              </a:gsLst>
-              <a:lin ang="5400000" scaled="0"/>
-            </a:gradFill>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="accent5">
-                  <a:shade val="95000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:dLbls>
-            <c:spPr>
-              <a:noFill/>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:txPr>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-                <a:spAutoFit/>
-              </a:bodyPr>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="50000"/>
-                        <a:lumOff val="50000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:endParaRPr lang="en-US"/>
-              </a:p>
-            </c:txPr>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="1"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:showBubbleSize val="0"/>
-            <c:showLeaderLines val="0"/>
-            <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
-                <c15:showLeaderLines val="1"/>
-                <c15:leaderLines>
-                  <c:spPr>
-                    <a:ln w="9525">
-                      <a:solidFill>
-                        <a:schemeClr val="tx1">
-                          <a:lumMod val="35000"/>
-                          <a:lumOff val="65000"/>
-                        </a:schemeClr>
-                      </a:solidFill>
-                    </a:ln>
-                    <a:effectLst/>
-                  </c:spPr>
-                </c15:leaderLines>
-              </c:ext>
-            </c:extLst>
-          </c:dLbls>
-          <c:cat>
-            <c:strRef>
-              <c:f>Sheet1!$M$7:$M$10</c:f>
-              <c:strCache>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>Bayes</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Tree</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Forest</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>KNN</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet1!$R$7:$R$10</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>0.208</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.321</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.319</c:v>
-                </c:pt>
-                <c:pt idx="3">
                   <c:v>0.321</c:v>
                 </c:pt>
               </c:numCache>
@@ -1479,13 +1294,13 @@
               <c:strCache>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>Bayes</c:v>
+                  <c:v>Naïve Bayes</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Tree</c:v>
+                  <c:v>Decision Tree</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>Forest</c:v>
+                  <c:v>Random Forest</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>KNN</c:v>
@@ -1606,13 +1421,13 @@
               <c:strCache>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>Bayes</c:v>
+                  <c:v>Naïve Bayes</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Tree</c:v>
+                  <c:v>Decision Tree</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>Forest</c:v>
+                  <c:v>Random Forest</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>KNN</c:v>
@@ -1734,13 +1549,13 @@
               <c:strCache>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>Bayes</c:v>
+                  <c:v>Naïve Bayes</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Tree</c:v>
+                  <c:v>Decision Tree</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>Forest</c:v>
+                  <c:v>Random Forest</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>KNN</c:v>
@@ -1861,13 +1676,13 @@
               <c:strCache>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>Bayes</c:v>
+                  <c:v>Naïve Bayes</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Tree</c:v>
+                  <c:v>Decision Tree</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>Forest</c:v>
+                  <c:v>Random Forest</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>KNN</c:v>
@@ -1988,13 +1803,13 @@
               <c:strCache>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>Bayes</c:v>
+                  <c:v>Naïve Bayes</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Tree</c:v>
+                  <c:v>Decision Tree</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>Forest</c:v>
+                  <c:v>Random Forest</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>KNN</c:v>
@@ -2115,13 +1930,13 @@
               <c:strCache>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>Bayes</c:v>
+                  <c:v>Naïve Bayes</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Tree</c:v>
+                  <c:v>Decision Tree</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>Forest</c:v>
+                  <c:v>Random Forest</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>KNN</c:v>
@@ -2955,44 +2770,39 @@
                     <a:lumOff val="50000"/>
                   </a:schemeClr>
                 </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
+                <a:latin typeface="Times New Roman" charset="0"/>
+                <a:ea typeface="Times New Roman" charset="0"/>
+                <a:cs typeface="Times New Roman" charset="0"/>
               </a:defRPr>
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>C</a:t>
+              <a:t>Comparison</a:t>
             </a:r>
             <a:r>
-              <a:rPr lang="en-US" altLang="zh-CN"/>
-              <a:t>omparison</a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="zh-CN" altLang="en-US" baseline="0"/>
+              <a:rPr lang="zh-CN"/>
               <a:t> </a:t>
             </a:r>
             <a:r>
-              <a:rPr lang="en-US" altLang="zh-CN" baseline="0"/>
+              <a:rPr lang="en-US"/>
               <a:t>between</a:t>
             </a:r>
             <a:r>
-              <a:rPr lang="zh-CN" altLang="en-US" baseline="0"/>
+              <a:rPr lang="zh-CN"/>
               <a:t> </a:t>
             </a:r>
             <a:r>
-              <a:rPr lang="en-US" altLang="zh-CN" baseline="0"/>
+              <a:rPr lang="en-US"/>
               <a:t>four</a:t>
             </a:r>
             <a:r>
-              <a:rPr lang="zh-CN" altLang="en-US" baseline="0"/>
+              <a:rPr lang="zh-CN"/>
               <a:t> </a:t>
             </a:r>
             <a:r>
-              <a:rPr lang="en-US" altLang="zh-CN" baseline="0"/>
+              <a:rPr lang="en-US"/>
               <a:t>classifier</a:t>
             </a:r>
-            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:rich>
       </c:tx>
@@ -3017,9 +2827,9 @@
                   <a:lumOff val="50000"/>
                 </a:schemeClr>
               </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
+              <a:latin typeface="Times New Roman" charset="0"/>
+              <a:ea typeface="Times New Roman" charset="0"/>
+              <a:cs typeface="Times New Roman" charset="0"/>
             </a:defRPr>
           </a:pPr>
           <a:endParaRPr lang="en-US"/>
@@ -3095,9 +2905,7 @@
               <a:effectLst/>
             </c:spPr>
             <c:txPr>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-                <a:spAutoFit/>
-              </a:bodyPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
@@ -3108,9 +2916,9 @@
                         <a:lumOff val="50000"/>
                       </a:schemeClr>
                     </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
+                    <a:latin typeface="Times New Roman" charset="0"/>
+                    <a:ea typeface="Times New Roman" charset="0"/>
+                    <a:cs typeface="Times New Roman" charset="0"/>
                   </a:defRPr>
                 </a:pPr>
                 <a:endParaRPr lang="en-US"/>
@@ -3150,13 +2958,13 @@
               <c:strCache>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>Bayes</c:v>
+                  <c:v>Naïve Bayes</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Tree</c:v>
+                  <c:v>Decision Tree</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>Forest</c:v>
+                  <c:v>Random Forest</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>KNN</c:v>
@@ -3247,9 +3055,7 @@
               <a:effectLst/>
             </c:spPr>
             <c:txPr>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-                <a:spAutoFit/>
-              </a:bodyPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
@@ -3260,9 +3066,9 @@
                         <a:lumOff val="50000"/>
                       </a:schemeClr>
                     </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
+                    <a:latin typeface="Times New Roman" charset="0"/>
+                    <a:ea typeface="Times New Roman" charset="0"/>
+                    <a:cs typeface="Times New Roman" charset="0"/>
                   </a:defRPr>
                 </a:pPr>
                 <a:endParaRPr lang="en-US"/>
@@ -3302,13 +3108,13 @@
               <c:strCache>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>Bayes</c:v>
+                  <c:v>Naïve Bayes</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Tree</c:v>
+                  <c:v>Decision Tree</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>Forest</c:v>
+                  <c:v>Random Forest</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>KNN</c:v>
@@ -3399,9 +3205,7 @@
               <a:effectLst/>
             </c:spPr>
             <c:txPr>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-                <a:spAutoFit/>
-              </a:bodyPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
@@ -3412,9 +3216,9 @@
                         <a:lumOff val="50000"/>
                       </a:schemeClr>
                     </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
+                    <a:latin typeface="Times New Roman" charset="0"/>
+                    <a:ea typeface="Times New Roman" charset="0"/>
+                    <a:cs typeface="Times New Roman" charset="0"/>
                   </a:defRPr>
                 </a:pPr>
                 <a:endParaRPr lang="en-US"/>
@@ -3454,13 +3258,13 @@
               <c:strCache>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>Bayes</c:v>
+                  <c:v>Naïve Bayes</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Tree</c:v>
+                  <c:v>Decision Tree</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>Forest</c:v>
+                  <c:v>Random Forest</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>KNN</c:v>
@@ -3539,9 +3343,9 @@
                     <a:lumOff val="50000"/>
                   </a:schemeClr>
                 </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
+                <a:latin typeface="Times New Roman" charset="0"/>
+                <a:ea typeface="Times New Roman" charset="0"/>
+                <a:cs typeface="Times New Roman" charset="0"/>
               </a:defRPr>
             </a:pPr>
             <a:endParaRPr lang="en-US"/>
@@ -3598,9 +3402,9 @@
                     <a:lumOff val="50000"/>
                   </a:schemeClr>
                 </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
+                <a:latin typeface="Times New Roman" charset="0"/>
+                <a:ea typeface="Times New Roman" charset="0"/>
+                <a:cs typeface="Times New Roman" charset="0"/>
               </a:defRPr>
             </a:pPr>
             <a:endParaRPr lang="en-US"/>
@@ -3641,9 +3445,9 @@
                   <a:lumOff val="50000"/>
                 </a:schemeClr>
               </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
+              <a:latin typeface="Times New Roman" charset="0"/>
+              <a:ea typeface="Times New Roman" charset="0"/>
+              <a:cs typeface="Times New Roman" charset="0"/>
             </a:defRPr>
           </a:pPr>
           <a:endParaRPr lang="en-US"/>
@@ -3674,7 +3478,11 @@
     <a:lstStyle/>
     <a:p>
       <a:pPr>
-        <a:defRPr/>
+        <a:defRPr>
+          <a:latin typeface="Times New Roman" charset="0"/>
+          <a:ea typeface="Times New Roman" charset="0"/>
+          <a:cs typeface="Times New Roman" charset="0"/>
+        </a:defRPr>
       </a:pPr>
       <a:endParaRPr lang="en-US"/>
     </a:p>
@@ -6315,53 +6123,53 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B6:R119"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A94" zoomScale="115" workbookViewId="0">
-      <selection activeCell="H119" sqref="H119"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="115" workbookViewId="0">
+      <selection activeCell="U17" sqref="U17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="6" spans="2:18" x14ac:dyDescent="0.2">
       <c r="C6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E6" t="s">
         <v>12</v>
       </c>
-      <c r="D6" t="s">
-        <v>14</v>
-      </c>
-      <c r="E6" t="s">
-        <v>15</v>
-      </c>
       <c r="F6" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="G6" t="s">
         <v>0</v>
       </c>
       <c r="H6" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="I6" t="s">
         <v>1</v>
       </c>
       <c r="N6" t="s">
+        <v>10</v>
+      </c>
+      <c r="O6" t="s">
         <v>13</v>
       </c>
-      <c r="O6" t="s">
-        <v>16</v>
-      </c>
       <c r="P6" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="Q6" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="R6" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="C7">
         <v>2.02</v>
@@ -6385,7 +6193,7 @@
         <v>0.67900000000000005</v>
       </c>
       <c r="M7" t="s">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="N7">
         <v>0.55339000000000005</v>
@@ -6405,7 +6213,7 @@
     </row>
     <row r="8" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="C8">
         <v>0.24</v>
@@ -6429,7 +6237,7 @@
         <v>0.67900000000000005</v>
       </c>
       <c r="M8" t="s">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="N8">
         <v>0.62078800000000001</v>
@@ -6449,7 +6257,7 @@
     </row>
     <row r="9" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B9" t="s">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="C9">
         <v>3.15</v>
@@ -6473,7 +6281,7 @@
         <v>0.73</v>
       </c>
       <c r="M9" t="s">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="N9">
         <v>0.62647200000000003</v>
@@ -6493,7 +6301,7 @@
     </row>
     <row r="10" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B10" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C10">
         <v>217.72</v>
@@ -6517,7 +6325,7 @@
         <v>0.73</v>
       </c>
       <c r="M10" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="N10">
         <v>0.62505100000000002</v>
@@ -6537,15 +6345,15 @@
     </row>
     <row r="55" spans="2:4" x14ac:dyDescent="0.2">
       <c r="C55" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D55" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
     <row r="56" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B56" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C56">
         <v>0.57799999999999996</v>
@@ -6556,7 +6364,7 @@
     </row>
     <row r="57" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B57" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C57">
         <v>0.621</v>
@@ -6567,10 +6375,10 @@
     </row>
     <row r="70" spans="2:5" x14ac:dyDescent="0.2">
       <c r="C70" t="s">
+        <v>10</v>
+      </c>
+      <c r="D70" t="s">
         <v>13</v>
-      </c>
-      <c r="D70" t="s">
-        <v>16</v>
       </c>
       <c r="E70" t="s">
         <v>1</v>
@@ -6578,7 +6386,7 @@
     </row>
     <row r="71" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B71" t="s">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="C71">
         <v>0.55339000000000005</v>
@@ -6592,7 +6400,7 @@
     </row>
     <row r="72" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B72" t="s">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="C72">
         <v>0.62078800000000001</v>
@@ -6606,7 +6414,7 @@
     </row>
     <row r="73" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B73" t="s">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="C73">
         <v>0.62647200000000003</v>
@@ -6620,7 +6428,7 @@
     </row>
     <row r="74" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B74" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C74">
         <v>0.62505100000000002</v>
@@ -6634,21 +6442,21 @@
     </row>
     <row r="101" spans="2:7" x14ac:dyDescent="0.2">
       <c r="D101" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E101" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="F101" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="G101" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="102" spans="2:7" x14ac:dyDescent="0.2">
       <c r="C102" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="D102">
         <v>2.02</v>
@@ -6665,7 +6473,7 @@
     </row>
     <row r="103" spans="2:7" x14ac:dyDescent="0.2">
       <c r="C103" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="D103">
         <v>0.54500000000000004</v>
@@ -6682,7 +6490,7 @@
     </row>
     <row r="104" spans="2:7" x14ac:dyDescent="0.2">
       <c r="C104" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="D104">
         <v>0.55300000000000005</v>
@@ -6699,7 +6507,7 @@
     </row>
     <row r="105" spans="2:7" x14ac:dyDescent="0.2">
       <c r="C105" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="D105">
         <v>0.5534</v>
@@ -6733,7 +6541,7 @@
     </row>
     <row r="107" spans="2:7" x14ac:dyDescent="0.2">
       <c r="C107" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="D107">
         <v>0.504</v>
@@ -6769,21 +6577,21 @@
     <row r="112" spans="2:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B112" s="3"/>
       <c r="C112" s="4" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="D112" s="4" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="E112" s="4" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="F112" s="4" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="113" spans="2:6" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B113" s="5" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C113" s="1">
         <v>2.02</v>
@@ -6817,7 +6625,7 @@
     </row>
     <row r="115" spans="2:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B115" s="5" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C115" s="1">
         <v>0.54500000000000004</v>
@@ -6834,7 +6642,7 @@
     </row>
     <row r="116" spans="2:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B116" s="6" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C116" s="2">
         <v>0.55300000000000005</v>
@@ -6851,7 +6659,7 @@
     </row>
     <row r="117" spans="2:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B117" s="5" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C117" s="1">
         <v>0.5534</v>
@@ -6868,7 +6676,7 @@
     </row>
     <row r="118" spans="2:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B118" s="6" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C118" s="2">
         <v>0.504</v>
@@ -6885,7 +6693,7 @@
     </row>
     <row r="119" spans="2:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B119" s="5" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C119" s="1">
         <v>0.67900000000000005</v>

</xml_diff>

<commit_message>
[KT proj2] -report done
</commit_message>
<xml_diff>
--- a/KTproj2/Reports/Charts.xlsx
+++ b/KTproj2/Reports/Charts.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="200" yWindow="460" windowWidth="38400" windowHeight="21060" tabRatio="500"/>
+    <workbookView xWindow="900" yWindow="6080" windowWidth="38400" windowHeight="21060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -38,19 +38,10 @@
     <t>KNN</t>
   </si>
   <si>
-    <t>Neg FM</t>
-  </si>
-  <si>
-    <t>Neu FM</t>
-  </si>
-  <si>
     <t>Accuracy</t>
   </si>
   <si>
     <t>Selected Attribute set</t>
-  </si>
-  <si>
-    <t>Positive FM</t>
   </si>
   <si>
     <t>Provided Attribute set</t>
@@ -93,6 +84,15 @@
   </si>
   <si>
     <t>Avg. ROC area</t>
+  </si>
+  <si>
+    <t>Positive F-Measure</t>
+  </si>
+  <si>
+    <t>Negative F-Measure</t>
+  </si>
+  <si>
+    <t>Neutral F-Measure</t>
   </si>
 </sst>
 </file>
@@ -386,7 +386,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>F-Measure</c:v>
+                  <c:v>Avg. F-Measure</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -531,7 +531,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Positive FM</c:v>
+                  <c:v>Positive F-Measure</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -676,7 +676,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Neg FM</c:v>
+                  <c:v>Negative F-Measure</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -821,7 +821,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Neu FM</c:v>
+                  <c:v>Neutral F-Measure</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1024,7 +1024,7 @@
         <c:axId val="-2095231936"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:min val="0.1"/>
+          <c:min val="0.25"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -6124,52 +6124,52 @@
   <dimension ref="B6:R119"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" zoomScale="115" workbookViewId="0">
-      <selection activeCell="U17" sqref="U17"/>
+      <selection activeCell="U24" sqref="U24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="6" spans="2:18" x14ac:dyDescent="0.2">
       <c r="C6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E6" t="s">
         <v>9</v>
       </c>
-      <c r="D6" t="s">
-        <v>11</v>
-      </c>
-      <c r="E6" t="s">
-        <v>12</v>
-      </c>
       <c r="F6" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="G6" t="s">
         <v>0</v>
       </c>
       <c r="H6" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="I6" t="s">
         <v>1</v>
       </c>
       <c r="N6" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="O6" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="P6" t="s">
-        <v>7</v>
+        <v>19</v>
       </c>
       <c r="Q6" t="s">
-        <v>3</v>
+        <v>20</v>
       </c>
       <c r="R6" t="s">
-        <v>4</v>
+        <v>21</v>
       </c>
     </row>
     <row r="7" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C7">
         <v>2.02</v>
@@ -6193,7 +6193,7 @@
         <v>0.67900000000000005</v>
       </c>
       <c r="M7" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="N7">
         <v>0.55339000000000005</v>
@@ -6213,7 +6213,7 @@
     </row>
     <row r="8" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C8">
         <v>0.24</v>
@@ -6237,7 +6237,7 @@
         <v>0.67900000000000005</v>
       </c>
       <c r="M8" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="N8">
         <v>0.62078800000000001</v>
@@ -6257,7 +6257,7 @@
     </row>
     <row r="9" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B9" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C9">
         <v>3.15</v>
@@ -6281,7 +6281,7 @@
         <v>0.73</v>
       </c>
       <c r="M9" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="N9">
         <v>0.62647200000000003</v>
@@ -6345,15 +6345,15 @@
     </row>
     <row r="55" spans="2:4" x14ac:dyDescent="0.2">
       <c r="C55" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D55" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="56" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B56" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C56">
         <v>0.57799999999999996</v>
@@ -6364,7 +6364,7 @@
     </row>
     <row r="57" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B57" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C57">
         <v>0.621</v>
@@ -6375,10 +6375,10 @@
     </row>
     <row r="70" spans="2:5" x14ac:dyDescent="0.2">
       <c r="C70" t="s">
+        <v>7</v>
+      </c>
+      <c r="D70" t="s">
         <v>10</v>
-      </c>
-      <c r="D70" t="s">
-        <v>13</v>
       </c>
       <c r="E70" t="s">
         <v>1</v>
@@ -6386,7 +6386,7 @@
     </row>
     <row r="71" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B71" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C71">
         <v>0.55339000000000005</v>
@@ -6400,7 +6400,7 @@
     </row>
     <row r="72" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B72" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C72">
         <v>0.62078800000000001</v>
@@ -6414,7 +6414,7 @@
     </row>
     <row r="73" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B73" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C73">
         <v>0.62647200000000003</v>
@@ -6442,13 +6442,13 @@
     </row>
     <row r="101" spans="2:7" x14ac:dyDescent="0.2">
       <c r="D101" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="E101" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="F101" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="G101" t="s">
         <v>2</v>
@@ -6456,7 +6456,7 @@
     </row>
     <row r="102" spans="2:7" x14ac:dyDescent="0.2">
       <c r="C102" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="D102">
         <v>2.02</v>
@@ -6473,7 +6473,7 @@
     </row>
     <row r="103" spans="2:7" x14ac:dyDescent="0.2">
       <c r="C103" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="D103">
         <v>0.54500000000000004</v>
@@ -6490,7 +6490,7 @@
     </row>
     <row r="104" spans="2:7" x14ac:dyDescent="0.2">
       <c r="C104" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="D104">
         <v>0.55300000000000005</v>
@@ -6507,7 +6507,7 @@
     </row>
     <row r="105" spans="2:7" x14ac:dyDescent="0.2">
       <c r="C105" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D105">
         <v>0.5534</v>
@@ -6541,7 +6541,7 @@
     </row>
     <row r="107" spans="2:7" x14ac:dyDescent="0.2">
       <c r="C107" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="D107">
         <v>0.504</v>
@@ -6577,13 +6577,13 @@
     <row r="112" spans="2:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B112" s="3"/>
       <c r="C112" s="4" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="D112" s="4" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E112" s="4" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="F112" s="4" t="s">
         <v>2</v>
@@ -6591,7 +6591,7 @@
     </row>
     <row r="113" spans="2:6" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B113" s="5" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C113" s="1">
         <v>2.02</v>
@@ -6625,7 +6625,7 @@
     </row>
     <row r="115" spans="2:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B115" s="5" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C115" s="1">
         <v>0.54500000000000004</v>
@@ -6642,7 +6642,7 @@
     </row>
     <row r="116" spans="2:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B116" s="6" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C116" s="2">
         <v>0.55300000000000005</v>
@@ -6659,7 +6659,7 @@
     </row>
     <row r="117" spans="2:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B117" s="5" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C117" s="1">
         <v>0.5534</v>
@@ -6676,7 +6676,7 @@
     </row>
     <row r="118" spans="2:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B118" s="6" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C118" s="2">
         <v>0.504</v>
@@ -6693,7 +6693,7 @@
     </row>
     <row r="119" spans="2:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B119" s="5" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C119" s="1">
         <v>0.67900000000000005</v>

</xml_diff>